<commit_message>
2023 - Day 13 - Solved parts I and II
</commit_message>
<xml_diff>
--- a/2023 - Python/Timing.xlsx
+++ b/2023 - Python/Timing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark_\Documents\GitHub\Advent-of-Code\2023 - Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D055FD15-F55F-4671-B716-D6B783B8D4DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6653101B-60C7-46BD-A889-D9BA6148CFCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{31D8ED60-C543-4761-8F44-FFA3DEE2EAE2}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -109,15 +109,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -133,6 +133,1303 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Advent of Code 2023</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$4:$D$5</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Part I</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Time (ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$6:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$6:$D$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3351-4C65-9BAF-4C2656027139}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$4:$E$5</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Part II</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Time (ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$6:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$6:$E$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3351-4C65-9BAF-4C2656027139}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="670698751"/>
+        <c:axId val="670699711"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="670698751"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Day</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-NL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="670699711"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="670699711"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-NL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="670698751"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>41910</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>306070</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{356C134E-45E7-4DA6-8340-18827E775856}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -434,8 +1731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2323E262-8313-4B12-BA60-03AD8357FF33}">
   <dimension ref="B2:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -446,11 +1743,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
@@ -655,9 +1952,15 @@
       <c r="C18" s="1">
         <v>13</v>
       </c>
+      <c r="D18">
+        <v>11</v>
+      </c>
+      <c r="E18">
+        <v>25</v>
+      </c>
       <c r="G18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
@@ -769,37 +2072,37 @@
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D32" s="4">
         <f>AVERAGE(D6:D30)</f>
-        <v>9.5727272727272723</v>
-      </c>
-      <c r="E32" s="5">
+        <v>9.6916666666666664</v>
+      </c>
+      <c r="E32" s="4">
         <f>AVERAGE(E6:E30)</f>
-        <v>11.018181818181818</v>
-      </c>
-      <c r="G32" s="3">
-        <f t="shared" si="0"/>
-        <v>20.59090909090909</v>
+        <v>12.183333333333332</v>
+      </c>
+      <c r="G32" s="2">
+        <f t="shared" si="0"/>
+        <v>21.875</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D34" s="5">
         <f>SUM(D6:D30)</f>
-        <v>105.3</v>
-      </c>
-      <c r="E34" s="6">
+        <v>116.3</v>
+      </c>
+      <c r="E34" s="5">
         <f>SUM(E6:E30)</f>
-        <v>121.2</v>
-      </c>
-      <c r="G34" s="3">
-        <f t="shared" si="0"/>
-        <v>226.5</v>
+        <v>146.19999999999999</v>
+      </c>
+      <c r="G34" s="2">
+        <f t="shared" si="0"/>
+        <v>262.5</v>
       </c>
     </row>
   </sheetData>
@@ -808,5 +2111,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2023 - Day 15 - Solved part I and II
</commit_message>
<xml_diff>
--- a/2023 - Python/Timing.xlsx
+++ b/2023 - Python/Timing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark_\Documents\GitHub\Advent-of-Code\2023 - Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6653101B-60C7-46BD-A889-D9BA6148CFCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D047AB72-64D3-4587-A0E7-4A5BCE598EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{31D8ED60-C543-4761-8F44-FFA3DEE2EAE2}"/>
   </bookViews>
@@ -363,6 +363,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1732,7 +1735,7 @@
   <dimension ref="B2:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1967,9 +1970,12 @@
       <c r="C19" s="1">
         <v>14</v>
       </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
       <c r="G19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
@@ -2077,7 +2083,7 @@
       </c>
       <c r="D32" s="4">
         <f>AVERAGE(D6:D30)</f>
-        <v>9.6916666666666664</v>
+        <v>9.1769230769230763</v>
       </c>
       <c r="E32" s="4">
         <f>AVERAGE(E6:E30)</f>
@@ -2085,7 +2091,7 @@
       </c>
       <c r="G32" s="2">
         <f t="shared" si="0"/>
-        <v>21.875</v>
+        <v>21.360256410256408</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.3">
@@ -2094,7 +2100,7 @@
       </c>
       <c r="D34" s="5">
         <f>SUM(D6:D30)</f>
-        <v>116.3</v>
+        <v>119.3</v>
       </c>
       <c r="E34" s="5">
         <f>SUM(E6:E30)</f>
@@ -2102,7 +2108,7 @@
       </c>
       <c r="G34" s="2">
         <f t="shared" si="0"/>
-        <v>262.5</v>
+        <v>265.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2023 - Updated timing day 14 part II
</commit_message>
<xml_diff>
--- a/2023 - Python/Timing.xlsx
+++ b/2023 - Python/Timing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark_\Documents\GitHub\Advent-of-Code\2023 - Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D047AB72-64D3-4587-A0E7-4A5BCE598EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F42AC32-6163-42DA-B746-F920910BF845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{31D8ED60-C543-4761-8F44-FFA3DEE2EAE2}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{31D8ED60-C543-4761-8F44-FFA3DEE2EAE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -367,6 +367,9 @@
                 <c:pt idx="13">
                   <c:v>3</c:v>
                 </c:pt>
+                <c:pt idx="14">
+                  <c:v>3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -528,6 +531,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -734,7 +740,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-NL"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1734,8 +1740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2323E262-8313-4B12-BA60-03AD8357FF33}">
   <dimension ref="B2:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1982,9 +1988,15 @@
       <c r="C20" s="1">
         <v>15</v>
       </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>7</v>
+      </c>
       <c r="G20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
@@ -2083,15 +2095,15 @@
       </c>
       <c r="D32" s="4">
         <f>AVERAGE(D6:D30)</f>
-        <v>9.1769230769230763</v>
+        <v>8.7357142857142858</v>
       </c>
       <c r="E32" s="4">
         <f>AVERAGE(E6:E30)</f>
-        <v>12.183333333333332</v>
+        <v>11.784615384615384</v>
       </c>
       <c r="G32" s="2">
         <f t="shared" si="0"/>
-        <v>21.360256410256408</v>
+        <v>20.520329670329669</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.3">
@@ -2100,15 +2112,15 @@
       </c>
       <c r="D34" s="5">
         <f>SUM(D6:D30)</f>
-        <v>119.3</v>
+        <v>122.3</v>
       </c>
       <c r="E34" s="5">
         <f>SUM(E6:E30)</f>
-        <v>146.19999999999999</v>
+        <v>153.19999999999999</v>
       </c>
       <c r="G34" s="2">
         <f t="shared" si="0"/>
-        <v>265.5</v>
+        <v>275.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2023 - Updated Timing.xlsx
</commit_message>
<xml_diff>
--- a/2023 - Python/Timing.xlsx
+++ b/2023 - Python/Timing.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark_\Documents\GitHub\Advent-of-Code\2023 - Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\mpeeters1\Documents\Advent of Code\2023 - Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F42AC32-6163-42DA-B746-F920910BF845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC3ED51-785E-491D-9142-976DEBF7923F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{31D8ED60-C543-4761-8F44-FFA3DEE2EAE2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{31D8ED60-C543-4761-8F44-FFA3DEE2EAE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -370,6 +370,15 @@
                 <c:pt idx="14">
                   <c:v>3</c:v>
                 </c:pt>
+                <c:pt idx="16">
+                  <c:v>2862</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -532,8 +541,20 @@
                 <c:pt idx="12">
                   <c:v>25</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>494</c:v>
+                </c:pt>
                 <c:pt idx="14">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9573</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -667,6 +688,7 @@
         <c:axId val="670699711"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1442,9 +1464,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1482,7 +1504,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1588,7 +1610,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1730,7 +1752,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1740,25 +1762,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2323E262-8313-4B12-BA60-03AD8357FF33}">
   <dimension ref="B2:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>2</v>
       </c>
@@ -1769,7 +1791,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>1</v>
       </c>
@@ -1783,7 +1805,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C6" s="1">
         <v>1</v>
       </c>
@@ -1798,7 +1820,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C7" s="1">
         <v>2</v>
       </c>
@@ -1813,7 +1835,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C8" s="1">
         <v>3</v>
       </c>
@@ -1828,7 +1850,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C9" s="1">
         <v>4</v>
       </c>
@@ -1843,7 +1865,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C10" s="1">
         <v>5</v>
       </c>
@@ -1858,7 +1880,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C11" s="1">
         <v>6</v>
       </c>
@@ -1873,7 +1895,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C12" s="1">
         <v>7</v>
       </c>
@@ -1888,7 +1910,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C13" s="1">
         <v>8</v>
       </c>
@@ -1903,7 +1925,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C14" s="1">
         <v>9</v>
       </c>
@@ -1918,7 +1940,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C15" s="1">
         <v>10</v>
       </c>
@@ -1933,7 +1955,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C16" s="1">
         <v>11</v>
       </c>
@@ -1948,7 +1970,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C17" s="1">
         <v>12</v>
       </c>
@@ -1957,7 +1979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C18" s="1">
         <v>13</v>
       </c>
@@ -1972,19 +1994,22 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C19" s="1">
         <v>14</v>
       </c>
       <c r="D19">
         <v>3</v>
       </c>
+      <c r="E19">
+        <v>494</v>
+      </c>
       <c r="G19">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C20" s="1">
         <v>15</v>
       </c>
@@ -1992,50 +2017,68 @@
         <v>3</v>
       </c>
       <c r="E20">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G20">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C21" s="1">
         <v>16</v>
       </c>
       <c r="G21">
-        <f t="shared" si="0"/>
+        <f>D21+E21</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C22" s="1">
         <v>17</v>
       </c>
+      <c r="D22">
+        <v>2862</v>
+      </c>
+      <c r="E22">
+        <v>9573</v>
+      </c>
       <c r="G22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+        <f>D22+E22</f>
+        <v>12435</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C23" s="1">
         <v>18</v>
       </c>
+      <c r="D23">
+        <v>0.8</v>
+      </c>
+      <c r="E23">
+        <v>0.8</v>
+      </c>
       <c r="G23">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C24" s="1">
         <v>19</v>
       </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
       <c r="G24">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C25" s="1">
         <v>20</v>
       </c>
@@ -2044,7 +2087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C26" s="1">
         <v>21</v>
       </c>
@@ -2053,7 +2096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C27" s="1">
         <v>22</v>
       </c>
@@ -2062,7 +2105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C28" s="1">
         <v>23</v>
       </c>
@@ -2071,7 +2114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C29" s="1">
         <v>24</v>
       </c>
@@ -2080,7 +2123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C30" s="1">
         <v>25</v>
       </c>
@@ -2089,38 +2132,38 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D32" s="4">
         <f>AVERAGE(D6:D30)</f>
-        <v>8.7357142857142858</v>
+        <v>175.8294117647059</v>
       </c>
       <c r="E32" s="4">
         <f>AVERAGE(E6:E30)</f>
-        <v>11.784615384615384</v>
+        <v>601.41176470588232</v>
       </c>
       <c r="G32" s="2">
         <f t="shared" si="0"/>
-        <v>20.520329670329669</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+        <v>777.24117647058824</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D34" s="5">
         <f>SUM(D6:D30)</f>
-        <v>122.3</v>
+        <v>2989.1000000000004</v>
       </c>
       <c r="E34" s="5">
         <f>SUM(E6:E30)</f>
-        <v>153.19999999999999</v>
+        <v>10224</v>
       </c>
       <c r="G34" s="2">
         <f t="shared" si="0"/>
-        <v>275.5</v>
+        <v>13213.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2023 - Day 16 - Solved part II
Runtime for part II is ~2 s
</commit_message>
<xml_diff>
--- a/2023 - Python/Timing.xlsx
+++ b/2023 - Python/Timing.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\mpeeters1\Documents\Advent of Code\2023 - Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark_\Documents\GitHub\Advent-of-Code\2023 - Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC3ED51-785E-491D-9142-976DEBF7923F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF62B1A-2B25-4017-ACF1-4797F83EAC66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{31D8ED60-C543-4761-8F44-FFA3DEE2EAE2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{31D8ED60-C543-4761-8F44-FFA3DEE2EAE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -370,6 +370,9 @@
                 <c:pt idx="14">
                   <c:v>3</c:v>
                 </c:pt>
+                <c:pt idx="15">
+                  <c:v>8</c:v>
+                </c:pt>
                 <c:pt idx="16">
                   <c:v>2862</c:v>
                 </c:pt>
@@ -546,6 +549,9 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1973</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>9573</c:v>
@@ -1464,9 +1470,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1504,7 +1510,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1610,7 +1616,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1752,7 +1758,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1762,25 +1768,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2323E262-8313-4B12-BA60-03AD8357FF33}">
   <dimension ref="B2:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
         <v>2</v>
       </c>
@@ -1791,7 +1797,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>1</v>
       </c>
@@ -1805,7 +1811,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C6" s="1">
         <v>1</v>
       </c>
@@ -1820,7 +1826,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C7" s="1">
         <v>2</v>
       </c>
@@ -1835,7 +1841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C8" s="1">
         <v>3</v>
       </c>
@@ -1850,7 +1856,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C9" s="1">
         <v>4</v>
       </c>
@@ -1865,7 +1871,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C10" s="1">
         <v>5</v>
       </c>
@@ -1880,7 +1886,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C11" s="1">
         <v>6</v>
       </c>
@@ -1895,7 +1901,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C12" s="1">
         <v>7</v>
       </c>
@@ -1910,7 +1916,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C13" s="1">
         <v>8</v>
       </c>
@@ -1925,7 +1931,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C14" s="1">
         <v>9</v>
       </c>
@@ -1940,7 +1946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C15" s="1">
         <v>10</v>
       </c>
@@ -1955,7 +1961,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C16" s="1">
         <v>11</v>
       </c>
@@ -1970,7 +1976,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C17" s="1">
         <v>12</v>
       </c>
@@ -1979,7 +1985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C18" s="1">
         <v>13</v>
       </c>
@@ -1994,7 +2000,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C19" s="1">
         <v>14</v>
       </c>
@@ -2009,7 +2015,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C20" s="1">
         <v>15</v>
       </c>
@@ -2024,16 +2030,22 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C21" s="1">
         <v>16</v>
       </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
+      <c r="E21">
+        <v>1973</v>
+      </c>
       <c r="G21">
         <f>D21+E21</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C22" s="1">
         <v>17</v>
       </c>
@@ -2048,7 +2060,7 @@
         <v>12435</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C23" s="1">
         <v>18</v>
       </c>
@@ -2063,7 +2075,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C24" s="1">
         <v>19</v>
       </c>
@@ -2078,7 +2090,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C25" s="1">
         <v>20</v>
       </c>
@@ -2087,7 +2099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C26" s="1">
         <v>21</v>
       </c>
@@ -2096,7 +2108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C27" s="1">
         <v>22</v>
       </c>
@@ -2105,7 +2117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C28" s="1">
         <v>23</v>
       </c>
@@ -2114,7 +2126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C29" s="1">
         <v>24</v>
       </c>
@@ -2123,7 +2135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C30" s="1">
         <v>25</v>
       </c>
@@ -2132,38 +2144,38 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B32" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D32" s="4">
         <f>AVERAGE(D6:D30)</f>
-        <v>175.8294117647059</v>
+        <v>166.50555555555559</v>
       </c>
       <c r="E32" s="4">
         <f>AVERAGE(E6:E30)</f>
-        <v>601.41176470588232</v>
+        <v>677.61111111111109</v>
       </c>
       <c r="G32" s="2">
         <f t="shared" si="0"/>
-        <v>777.24117647058824</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+        <v>844.11666666666667</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D34" s="5">
         <f>SUM(D6:D30)</f>
-        <v>2989.1000000000004</v>
+        <v>2997.1000000000004</v>
       </c>
       <c r="E34" s="5">
         <f>SUM(E6:E30)</f>
-        <v>10224</v>
+        <v>12197</v>
       </c>
       <c r="G34" s="2">
         <f t="shared" si="0"/>
-        <v>13213.1</v>
+        <v>15194.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2023 - Timing.xlsx updated
</commit_message>
<xml_diff>
--- a/2023 - Python/Timing.xlsx
+++ b/2023 - Python/Timing.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark_\Documents\GitHub\Advent-of-Code\2023 - Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\mpeeters1\Documents\Advent of Code\2023 - Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2779785E-DA06-4A12-BB65-6731EE7EB113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784C831C-9CF4-4474-BCDD-3FF6C33FF23E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{31D8ED60-C543-4761-8F44-FFA3DEE2EAE2}"/>
+    <workbookView xWindow="5850" yWindow="2085" windowWidth="14430" windowHeight="9960" xr2:uid="{31D8ED60-C543-4761-8F44-FFA3DEE2EAE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -381,6 +381,9 @@
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>94</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1470,9 +1473,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1510,7 +1513,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1616,7 +1619,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1758,7 +1761,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1768,25 +1771,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2323E262-8313-4B12-BA60-03AD8357FF33}">
   <dimension ref="B2:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>2</v>
       </c>
@@ -1797,7 +1800,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>1</v>
       </c>
@@ -1811,7 +1814,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C6" s="1">
         <v>1</v>
       </c>
@@ -1826,7 +1829,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C7" s="1">
         <v>2</v>
       </c>
@@ -1841,7 +1844,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C8" s="1">
         <v>3</v>
       </c>
@@ -1856,7 +1859,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C9" s="1">
         <v>4</v>
       </c>
@@ -1871,7 +1874,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C10" s="1">
         <v>5</v>
       </c>
@@ -1886,7 +1889,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C11" s="1">
         <v>6</v>
       </c>
@@ -1901,7 +1904,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C12" s="1">
         <v>7</v>
       </c>
@@ -1916,7 +1919,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C13" s="1">
         <v>8</v>
       </c>
@@ -1931,7 +1934,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C14" s="1">
         <v>9</v>
       </c>
@@ -1946,7 +1949,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C15" s="1">
         <v>10</v>
       </c>
@@ -1961,7 +1964,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C16" s="1">
         <v>11</v>
       </c>
@@ -1976,7 +1979,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C17" s="1">
         <v>12</v>
       </c>
@@ -1985,7 +1988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C18" s="1">
         <v>13</v>
       </c>
@@ -2000,7 +2003,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C19" s="1">
         <v>14</v>
       </c>
@@ -2015,7 +2018,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C20" s="1">
         <v>15</v>
       </c>
@@ -2030,7 +2033,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C21" s="1">
         <v>16</v>
       </c>
@@ -2045,7 +2048,7 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C22" s="1">
         <v>17</v>
       </c>
@@ -2060,7 +2063,7 @@
         <v>12435</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C23" s="1">
         <v>18</v>
       </c>
@@ -2075,7 +2078,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C24" s="1">
         <v>19</v>
       </c>
@@ -2090,16 +2093,19 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C25" s="1">
         <v>20</v>
       </c>
+      <c r="D25">
+        <v>94</v>
+      </c>
       <c r="G25">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C26" s="1">
         <v>21</v>
       </c>
@@ -2108,7 +2114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C27" s="1">
         <v>22</v>
       </c>
@@ -2117,7 +2123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C28" s="1">
         <v>23</v>
       </c>
@@ -2126,7 +2132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C29" s="1">
         <v>24</v>
       </c>
@@ -2135,7 +2141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C30" s="1">
         <v>25</v>
       </c>
@@ -2144,13 +2150,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D32" s="4">
         <f>AVERAGE(D6:D30)</f>
-        <v>166.50555555555559</v>
+        <v>162.68947368421055</v>
       </c>
       <c r="E32" s="4">
         <f>AVERAGE(E6:E30)</f>
@@ -2158,16 +2164,16 @@
       </c>
       <c r="G32" s="2">
         <f t="shared" si="0"/>
-        <v>844.11666666666667</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+        <v>840.30058479532158</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D34" s="5">
         <f>SUM(D6:D30)</f>
-        <v>2997.1000000000004</v>
+        <v>3091.1000000000004</v>
       </c>
       <c r="E34" s="5">
         <f>SUM(E6:E30)</f>
@@ -2175,7 +2181,7 @@
       </c>
       <c r="G34" s="2">
         <f t="shared" si="0"/>
-        <v>15194.1</v>
+        <v>15288.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>